<commit_message>
more edits to file information
</commit_message>
<xml_diff>
--- a/NPS TEMPLATE-SCPN.xlsx
+++ b/NPS TEMPLATE-SCPN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__MyWorkSpace\IT-NPGallery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aerlewine\Documents\ThumbsPlusPhotos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70716847-2041-41F1-95E6-870CE6F9B7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FB803F-C344-46DD-8F36-9E6E6ADB4ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="273" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27060" yWindow="-150" windowWidth="20790" windowHeight="13350" tabRatio="273" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NPS Photo Metadata" sheetId="2" r:id="rId1"/>
@@ -1590,7 +1590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{FC34683B-72E6-474D-A911-B46D1E6F10B8}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{FC34683B-72E6-474D-A911-B46D1E6F10B8}">
       <text>
         <r>
           <rPr>
@@ -1618,7 +1618,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{F2514504-D587-42D6-80DB-8FD200E8614A}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{F2514504-D587-42D6-80DB-8FD200E8614A}">
       <text>
         <r>
           <rPr>
@@ -1642,7 +1642,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{244A95DA-2788-46B9-A94C-5E8A5224DA52}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{244A95DA-2788-46B9-A94C-5E8A5224DA52}">
       <text>
         <r>
           <rPr>
@@ -1703,7 +1703,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{B67A7031-6ED9-415B-98B8-586AC9F57F0E}">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{B67A7031-6ED9-415B-98B8-586AC9F57F0E}">
       <text>
         <r>
           <rPr>
@@ -1727,7 +1727,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{8D932CF0-80C7-4A78-B969-AD7C0C28D320}">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{8D932CF0-80C7-4A78-B969-AD7C0C28D320}">
       <text>
         <r>
           <rPr>
@@ -1751,7 +1751,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{FC43CBE3-6C4F-43C5-A344-3623DE8D864D}">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{FC43CBE3-6C4F-43C5-A344-3623DE8D864D}">
       <text>
         <r>
           <rPr>
@@ -1823,7 +1823,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{46E3A0A8-01B0-4B81-A9D4-8BCBA490EBBB}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{46E3A0A8-01B0-4B81-A9D4-8BCBA490EBBB}">
       <text>
         <r>
           <rPr>
@@ -1847,7 +1847,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{57FA5E90-BC54-41C2-AB87-EBDC1A9824CC}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{57FA5E90-BC54-41C2-AB87-EBDC1A9824CC}">
       <text>
         <r>
           <rPr>
@@ -1871,7 +1871,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{9F7FD720-1C56-49EF-9BD3-E838A2EA9C25}">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{9F7FD720-1C56-49EF-9BD3-E838A2EA9C25}">
       <text>
         <r>
           <rPr>
@@ -1905,7 +1905,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="1" shapeId="0" xr:uid="{3C01DD7C-464F-4692-8AD2-18510E90622C}">
+    <comment ref="A14" authorId="1" shapeId="0" xr:uid="{3C01DD7C-464F-4692-8AD2-18510E90622C}">
       <text>
         <r>
           <rPr>
@@ -1928,7 +1928,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="1" shapeId="0" xr:uid="{055CDC42-E1A3-47BF-A861-D17F0CA01D46}">
+    <comment ref="A15" authorId="1" shapeId="0" xr:uid="{055CDC42-E1A3-47BF-A861-D17F0CA01D46}">
       <text>
         <r>
           <rPr>
@@ -1962,7 +1962,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="1" shapeId="0" xr:uid="{DD97503E-3054-4511-AD56-B6827E02FBD9}">
+    <comment ref="A16" authorId="1" shapeId="0" xr:uid="{DD97503E-3054-4511-AD56-B6827E02FBD9}">
       <text>
         <r>
           <rPr>
@@ -1995,7 +1995,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="1" shapeId="0" xr:uid="{46760A89-1182-47F9-BBC1-F392E6A1988F}">
+    <comment ref="A17" authorId="1" shapeId="0" xr:uid="{46760A89-1182-47F9-BBC1-F392E6A1988F}">
       <text>
         <r>
           <rPr>
@@ -2028,7 +2028,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{DA91C43F-BA08-43A1-9049-9080893600E3}">
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{DA91C43F-BA08-43A1-9049-9080893600E3}">
       <text>
         <r>
           <rPr>
@@ -2089,7 +2089,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="1" shapeId="0" xr:uid="{6148DCD1-96E6-43E6-AB9E-38E6684059BE}">
+    <comment ref="A19" authorId="1" shapeId="0" xr:uid="{6148DCD1-96E6-43E6-AB9E-38E6684059BE}">
       <text>
         <r>
           <rPr>
@@ -2112,7 +2112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A17" authorId="1" shapeId="0" xr:uid="{B71CA8FB-6FB1-4805-B048-99C2EBBFD739}">
+    <comment ref="A20" authorId="1" shapeId="0" xr:uid="{B71CA8FB-6FB1-4805-B048-99C2EBBFD739}">
       <text>
         <r>
           <rPr>
@@ -2145,7 +2145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="1" shapeId="0" xr:uid="{9396C68C-7539-4EE0-A2DC-01C882BBEE0A}">
+    <comment ref="A21" authorId="1" shapeId="0" xr:uid="{9396C68C-7539-4EE0-A2DC-01C882BBEE0A}">
       <text>
         <r>
           <rPr>
@@ -2168,7 +2168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{A3ACD5B9-4572-4799-AB9F-A2CD576DFEB3}">
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{A3ACD5B9-4572-4799-AB9F-A2CD576DFEB3}">
       <text>
         <r>
           <rPr>
@@ -2192,7 +2192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="1" shapeId="0" xr:uid="{F6AF2052-DFE5-49AE-A694-6BFCADF186FD}">
+    <comment ref="A23" authorId="1" shapeId="0" xr:uid="{F6AF2052-DFE5-49AE-A694-6BFCADF186FD}">
       <text>
         <r>
           <rPr>
@@ -2215,7 +2215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="1" shapeId="0" xr:uid="{B1F5E062-015C-4456-8C2F-6C4545AD0FA6}">
+    <comment ref="A24" authorId="1" shapeId="0" xr:uid="{B1F5E062-015C-4456-8C2F-6C4545AD0FA6}">
       <text>
         <r>
           <rPr>
@@ -2238,7 +2238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="1" shapeId="0" xr:uid="{66B851C9-3313-4EE6-9F3E-943E069FCCD2}">
+    <comment ref="A25" authorId="1" shapeId="0" xr:uid="{66B851C9-3313-4EE6-9F3E-943E069FCCD2}">
       <text>
         <r>
           <rPr>
@@ -2261,7 +2261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="1" shapeId="0" xr:uid="{AE4D5ACC-35B4-498A-A7BD-9C944D1518EC}">
+    <comment ref="A26" authorId="1" shapeId="0" xr:uid="{AE4D5ACC-35B4-498A-A7BD-9C944D1518EC}">
       <text>
         <r>
           <rPr>
@@ -2284,7 +2284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A24" authorId="1" shapeId="0" xr:uid="{F515915A-CE1C-4547-BA29-6ACB6656BD50}">
+    <comment ref="A27" authorId="1" shapeId="0" xr:uid="{F515915A-CE1C-4547-BA29-6ACB6656BD50}">
       <text>
         <r>
           <rPr>
@@ -2307,7 +2307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="1" shapeId="0" xr:uid="{F5BF7485-6160-4146-8000-67632AFAA6CA}">
+    <comment ref="A28" authorId="1" shapeId="0" xr:uid="{F5BF7485-6160-4146-8000-67632AFAA6CA}">
       <text>
         <r>
           <rPr>
@@ -2335,7 +2335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="143">
   <si>
     <t>Title</t>
   </si>
@@ -2763,6 +2763,27 @@
   <si>
     <t>title case</t>
   </si>
+  <si>
+    <t>added - idThumb</t>
+  </si>
+  <si>
+    <t>idThumb</t>
+  </si>
+  <si>
+    <t>added - filePath</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <t>added - photoNumber</t>
+  </si>
+  <si>
+    <t>photoNumber</t>
+  </si>
+  <si>
+    <t>Folder name / uf_photoDate</t>
+  </si>
 </sst>
 </file>
 
@@ -2837,7 +2858,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2892,6 +2913,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2905,7 +2932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2941,6 +2968,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3891,10 +3919,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0385044-074C-4447-B588-5C002A577DD0}">
-  <dimension ref="A1:C16384"/>
+  <dimension ref="A1:C16387"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3904,7 +3932,7 @@
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
@@ -3912,200 +3940,215 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
         <v>134</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
-        <v>121</v>
+      <c r="B6" t="s">
+        <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B9" s="28" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>130</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-    </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
     </row>
@@ -53161,6 +53204,15 @@
     </row>
     <row r="16384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16384" s="5"/>
+    </row>
+    <row r="16385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16385" s="5"/>
+    </row>
+    <row r="16386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16386" s="5"/>
+    </row>
+    <row r="16387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16387" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53169,18 +53221,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53298,14 +53350,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241A4E59-BC2C-43AF-B0E8-1D76C3356527}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E46C7101-2896-4512-8963-4B1F206A1171}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -53316,6 +53360,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241A4E59-BC2C-43AF-B0E8-1D76C3356527}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>